<commit_message>
add data for Karma experiments
</commit_message>
<xml_diff>
--- a/casestudy/karma-4/KarmaExperiments.xlsx
+++ b/casestudy/karma-4/KarmaExperiments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franktip/git/mutation-testing-data/bugs.js-study/Karma/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franktip/git/mutation-testing-data/casestudy/karma-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F58838-69AC-6943-9106-4800B14B695D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DFD11B-184C-A346-AB0B-BAF7CD46E1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6660" yWindow="3440" windowWidth="28040" windowHeight="17440" xr2:uid="{4FE0EC7D-01FA-454F-B2A5-BE08A4EE20E2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="28">
   <si>
     <t>bug#</t>
   </si>
@@ -223,6 +223,15 @@
     "completionId": 0,
     "reason": "if/test"
   }</t>
+  </si>
+  <si>
+    <t>10 test failures, all different from the one caused by the original bug</t>
+  </si>
+  <si>
+    <t>11 test failures, of which 1 is the same as the failure caused by the original bug</t>
+  </si>
+  <si>
+    <t>same test failure as the one caused by the original bug</t>
   </si>
 </sst>
 </file>
@@ -358,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -461,9 +470,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -832,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C302C4E-966E-E54E-A26B-052C43363DBC}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M4" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -852,7 +858,7 @@
     <col min="13" max="13" width="88" customWidth="1"/>
     <col min="14" max="14" width="24.5" customWidth="1"/>
     <col min="15" max="15" width="15.5" customWidth="1"/>
-    <col min="16" max="16" width="110.83203125" customWidth="1"/>
+    <col min="16" max="16" width="64.83203125" customWidth="1"/>
     <col min="17" max="17" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -864,30 +870,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1"/>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="48" t="s">
+      <c r="E1" s="46"/>
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="42" t="s">
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="44" t="s">
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="43" t="s">
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="3"/>
@@ -937,10 +943,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="196" customHeight="1">
-      <c r="A3" s="46">
+      <c r="A3" s="45">
         <v>4</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="44" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="14">
@@ -958,32 +964,40 @@
       <c r="G3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="18"/>
+      <c r="H3" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="I3" s="27">
         <v>1</v>
       </c>
       <c r="J3" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="12"/>
+      <c r="K3" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="L3" s="35">
         <v>1</v>
       </c>
       <c r="M3" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="34"/>
+      <c r="N3" s="34" t="s">
+        <v>25</v>
+      </c>
       <c r="O3" s="36">
         <v>1</v>
       </c>
       <c r="P3" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="38"/>
+      <c r="Q3" s="40" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:17" ht="223" customHeight="1">
-      <c r="A4" s="46"/>
-      <c r="B4" s="45"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="14">
         <v>2</v>
       </c>
@@ -999,7 +1013,9 @@
       <c r="G4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="18"/>
+      <c r="H4" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="I4" s="28">
         <v>2</v>
       </c>
@@ -1015,18 +1031,22 @@
       <c r="M4" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="34"/>
+      <c r="N4" s="34" t="s">
+        <v>26</v>
+      </c>
       <c r="O4" s="36">
         <v>2</v>
       </c>
       <c r="P4" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="39"/>
+      <c r="Q4" s="40" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:17" ht="217" customHeight="1">
-      <c r="A5" s="46"/>
-      <c r="B5" s="45"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="14">
         <v>3</v>
       </c>
@@ -1042,7 +1062,9 @@
       <c r="G5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="18"/>
+      <c r="H5" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="I5" s="28" t="s">
         <v>2</v>
       </c>
@@ -1065,11 +1087,13 @@
       <c r="P5" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="Q5" s="38"/>
+      <c r="Q5" s="40" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="169" customHeight="1">
-      <c r="A6" s="46"/>
-      <c r="B6" s="45"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
@@ -1096,7 +1120,7 @@
         <v>2</v>
       </c>
       <c r="P6" s="37"/>
-      <c r="Q6" s="39"/>
+      <c r="Q6" s="38"/>
     </row>
     <row r="7" spans="1:17" ht="157" customHeight="1">
       <c r="A7" s="4"/>
@@ -1127,7 +1151,7 @@
         <v>5</v>
       </c>
       <c r="P7" s="37"/>
-      <c r="Q7" s="39"/>
+      <c r="Q7" s="38"/>
     </row>
     <row r="8" spans="1:17" ht="168" customHeight="1">
       <c r="A8" s="4"/>
@@ -1156,7 +1180,7 @@
         <v>6</v>
       </c>
       <c r="P8" s="37"/>
-      <c r="Q8" s="40"/>
+      <c r="Q8" s="39"/>
     </row>
     <row r="9" spans="1:17" ht="150" customHeight="1">
       <c r="A9" s="4"/>
@@ -1184,8 +1208,8 @@
       <c r="O9" s="36">
         <v>7</v>
       </c>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="39"/>
     </row>
     <row r="10" spans="1:17" ht="22">
       <c r="A10" s="4"/>
@@ -1213,8 +1237,8 @@
       <c r="O10" s="36">
         <v>8</v>
       </c>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="39"/>
     </row>
     <row r="11" spans="1:17" ht="22">
       <c r="A11" s="4"/>
@@ -1242,8 +1266,8 @@
       <c r="O11" s="36">
         <v>9</v>
       </c>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="39"/>
     </row>
     <row r="12" spans="1:17" ht="22">
       <c r="A12" s="4"/>
@@ -1271,8 +1295,8 @@
       <c r="O12" s="36">
         <v>10</v>
       </c>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="39"/>
     </row>
     <row r="13" spans="1:17" ht="22">
       <c r="A13" s="4"/>
@@ -1300,8 +1324,8 @@
       <c r="O13" s="36">
         <v>11</v>
       </c>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="39"/>
     </row>
     <row r="14" spans="1:17" ht="22">
       <c r="A14" s="4"/>

</xml_diff>

<commit_message>
add data for karma-4
</commit_message>
<xml_diff>
--- a/casestudy/karma-4/KarmaExperiments.xlsx
+++ b/casestudy/karma-4/KarmaExperiments.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franktip/git/mutation-testing-data/casestudy/karma-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DFD11B-184C-A346-AB0B-BAF7CD46E1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CBA3F8-2308-E641-9EF6-2A2A40B47283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="3440" windowWidth="28040" windowHeight="17440" xr2:uid="{4FE0EC7D-01FA-454F-B2A5-BE08A4EE20E2}"/>
+    <workbookView xWindow="6660" yWindow="3440" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{4FE0EC7D-01FA-454F-B2A5-BE08A4EE20E2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bug 4" sheetId="1" r:id="rId1"/>
+    <sheet name="bug" sheetId="2" r:id="rId1"/>
+    <sheet name="mutants" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="42">
   <si>
     <t>bug#</t>
   </si>
@@ -126,15 +127,6 @@
   }</t>
   </si>
   <si>
-    <t>Same as the original bug</t>
-  </si>
-  <si>
-    <t>Same behavior as the fixed version; a surviving mutant</t>
-  </si>
-  <si>
-    <t>Multiple different failures</t>
-  </si>
-  <si>
     <t xml:space="preserve"> {
     "file": "lib/reporter.js",
     "startLine": 55,
@@ -163,9 +155,6 @@
   }</t>
   </si>
   <si>
-    <t>multiple different failures</t>
-  </si>
-  <si>
     <t xml:space="preserve"> {
     "file": "lib/reporter.js",
     "startLine": 55,
@@ -232,6 +221,351 @@
   </si>
   <si>
     <t>same test failure as the one caused by the original bug</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>buggy code</t>
+  </si>
+  <si>
+    <t>fixed code</t>
+  </si>
+  <si>
+    <t>test failures</t>
+  </si>
+  <si>
+    <t>lib/reporter.js</t>
+  </si>
+  <si>
+    <t>file &amp;&amp; file.sourceMap &amp;&amp; line</t>
+  </si>
+  <si>
+    <t>file &amp;&amp; file.sourceMap</t>
+  </si>
+  <si>
+    <t>1) reporter
+       formatError
+         source maps
+           should not try to use source maps when no line is given:
+      Uncaught AssertionError: expected 'at /original/b.js:3 &lt;- b.js\n' to equal 'at b.js\n'
+      + expected - actual
+      -at /original/b.js:3 &lt;- b.js
+      +at b.js
+      at test/unit/reporter.spec.js:333:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)</t>
+  </si>
+  <si>
+    <t>run tests using: npm run test:unit</t>
+  </si>
+  <si>
+    <t>This is  the original bug!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10 failing
+  1) reporter
+       formatError
+         source maps
+           should rewrite stack traces:
+      Uncaught AssertionError: expected 'at b.js:2:6\n' to equal 'at /original/b.js:4:8 &lt;- b.js:2:6\n'
+      + expected - actual
+      -at b.js:2:6
+      +at /original/b.js:4:8 &lt;- b.js:2:6
+      at test/unit/reporter.spec.js:198:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  2) reporter
+       formatError
+         source maps
+           should handle source map errors gracefully:
+      Uncaught AssertionError: expected 0 to equal 2
+      + expected - actual
+      -0
+      +2
+      at test/unit/reporter.spec.js:219:44
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  3) reporter
+       formatError
+         source maps
+           should rewrite stack traces (when basePath is empty):
+      Uncaught AssertionError: expected 'at b.js:2:6\n' to equal 'at /original/b.js:4:8 &lt;- b.js:2:6\n'
+      + expected - actual
+      -at b.js:2:6
+      +at /original/b.js:4:8 &lt;- b.js:2:6
+      at test/unit/reporter.spec.js:258:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  4) reporter
+       formatError
+         source maps
+           should rewrite stack traces to the first column when no column is given:
+      Uncaught AssertionError: expected 'at b.js:2\n' to equal 'at /original/b.js:4:3 &lt;- b.js:2\n'
+      + expected - actual
+      -at b.js:2
+      +at /original/b.js:4:3 &lt;- b.js:2
+      at test/unit/reporter.spec.js:273:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  5) reporter
+       formatError
+         source maps
+           should rewrite relative url stack traces:
+      Uncaught AssertionError: expected 'at b.js:2:6\n' to equal 'at /original/b.js:4:8 &lt;- b.js:2:6\n'
+      + expected - actual
+      -at b.js:2:6
+      +at /original/b.js:4:8 &lt;- b.js:2:6
+      at test/unit/reporter.spec.js:288:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  6) reporter
+       formatError
+         source maps
+           should resolve relative urls from source maps:
+      Uncaught AssertionError: expected 'at path/a.js:2:6\n' to equal 'at path/original/a.fancyjs:4:8 &lt;- path/a.js:2:6\n'
+      + expected - actual
+      -at path/a.js:2:6
+      +at path/original/a.fancyjs:4:8 &lt;- path/a.js:2:6
+      at test/unit/reporter.spec.js:303:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  7) reporter
+       formatError
+         source maps
+           should fall back to non-source-map format if originalPositionFor throws:
+      Uncaught AssertionError: expected 'at b.js:0:0\n' to equal 'at b.js\n'
+      + expected - actual
+      -at b.js:0:0
+      +at b.js
+      at test/unit/reporter.spec.js:318:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  8) reporter
+       formatError
+         source maps
+           should not try to match domains with spaces:
+      Uncaught AssertionError: expected '"http://localhost:9876"\n at b.js:2:6\n' to equal '"http://localhost:9876"\n at /original/b.js:4:8 &lt;- b.js:2:6\n'
+      + expected - actual
+       "http://localhost:9876"
+      - at b.js:2:6
+      + at /original/b.js:4:8 &lt;- b.js:2:6
+      at test/unit/reporter.spec.js:349:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  9) reporter
+       formatError
+         source maps
+           Windows
+             should correct rewrite stack traces without sha:
+      Uncaught AssertionError: expected 'at C:/a/b/c.js:2:6\n' to equal 'at c:/original/b.js:4:8 &lt;- C:/a/b/c.js:2:6\n'
+      + expected - actual
+      -at C:/a/b/c.js:2:6
+      +at c:/original/b.js:4:8 &lt;- C:/a/b/c.js:2:6
+      at test/unit/reporter.spec.js:369:43
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  10) reporter
+       formatError
+         source maps
+           Windows
+             should correct rewrite stack traces with sha:
+      Uncaught AssertionError: expected 'at C:/a/b/c.js:2:6\n' to equal 'at c:/original/b.js:4:8 &lt;- C:/a/b/c.js:2:6\n'
+      + expected - actual
+      -at C:/a/b/c.js:2:6
+      +at c:/original/b.js:4:8 &lt;- C:/a/b/c.js:2:6
+      at test/unit/reporter.spec.js:379:43
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)</t>
+  </si>
+  <si>
+    <t>10 test  failures, all different from the one caused by the original bug</t>
+  </si>
+  <si>
+    <t>surviving mutant -- does not cause any test failures</t>
+  </si>
+  <si>
+    <t>11 failing
+  1) reporter
+       formatError
+         source maps
+           should rewrite stack traces:
+      Uncaught AssertionError: expected 'at b.js:2:6\n' to equal 'at /original/b.js:4:8 &lt;- b.js:2:6\n'
+      + expected - actual
+      -at b.js:2:6
+      +at /original/b.js:4:8 &lt;- b.js:2:6
+      at test/unit/reporter.spec.js:198:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  2) reporter
+       formatError
+         source maps
+           should handle source map errors gracefully:
+      Uncaught AssertionError: expected 0 to equal 2
+      + expected - actual
+      -0
+      +2
+      at test/unit/reporter.spec.js:219:44
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  3) reporter
+       formatError
+         source maps
+           should rewrite stack traces (when basePath is empty):
+      Uncaught AssertionError: expected 'at b.js:2:6\n' to equal 'at /original/b.js:4:8 &lt;- b.js:2:6\n'
+      + expected - actual
+      -at b.js:2:6
+      +at /original/b.js:4:8 &lt;- b.js:2:6
+      at test/unit/reporter.spec.js:258:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  4) reporter
+       formatError
+         source maps
+           should rewrite stack traces to the first column when no column is given:
+      Uncaught AssertionError: expected 'at b.js:2\n' to equal 'at /original/b.js:4:3 &lt;- b.js:2\n'
+      + expected - actual
+      -at b.js:2
+      +at /original/b.js:4:3 &lt;- b.js:2
+      at test/unit/reporter.spec.js:273:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  5) reporter
+       formatError
+         source maps
+           should rewrite relative url stack traces:
+      Uncaught AssertionError: expected 'at b.js:2:6\n' to equal 'at /original/b.js:4:8 &lt;- b.js:2:6\n'
+      + expected - actual
+      -at b.js:2:6
+      +at /original/b.js:4:8 &lt;- b.js:2:6
+      at test/unit/reporter.spec.js:288:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  6) reporter
+       formatError
+         source maps
+           should resolve relative urls from source maps:
+      Uncaught AssertionError: expected 'at path/a.js:2:6\n' to equal 'at path/original/a.fancyjs:4:8 &lt;- path/a.js:2:6\n'
+      + expected - actual
+      -at path/a.js:2:6
+      +at path/original/a.fancyjs:4:8 &lt;- path/a.js:2:6
+      at test/unit/reporter.spec.js:303:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  7) reporter
+       formatError
+         source maps
+           should fall back to non-source-map format if originalPositionFor throws:
+      Uncaught AssertionError: expected 'at b.js:0:0\n' to equal 'at b.js\n'
+      + expected - actual
+      -at b.js:0:0
+      +at b.js
+      at test/unit/reporter.spec.js:318:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  8) reporter
+       formatError
+         source maps
+           should not try to use source maps when no line is given:
+      Uncaught AssertionError: expected 'at /original/b.js:3 &lt;- b.js\n' to equal 'at b.js\n'
+      + expected - actual
+      -at /original/b.js:3 &lt;- b.js
+      +at b.js
+      at test/unit/reporter.spec.js:333:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  9) reporter
+       formatError
+         source maps
+           should not try to match domains with spaces:
+      Uncaught AssertionError: expected '"http://localhost:9876"\n at b.js:2:6\n' to equal '"http://localhost:9876"\n at /original/b.js:4:8 &lt;- b.js:2:6\n'
+      + expected - actual
+       "http://localhost:9876"
+      - at b.js:2:6
+      + at /original/b.js:4:8 &lt;- b.js:2:6
+      at test/unit/reporter.spec.js:349:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  10) reporter
+       formatError
+         source maps
+           Windows
+             should correct rewrite stack traces without sha:
+      Uncaught AssertionError: expected 'at C:/a/b/c.js:2:6\n' to equal 'at c:/original/b.js:4:8 &lt;- C:/a/b/c.js:2:6\n'
+      + expected - actual
+      -at C:/a/b/c.js:2:6
+      +at c:/original/b.js:4:8 &lt;- C:/a/b/c.js:2:6
+      at test/unit/reporter.spec.js:369:43
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)
+  11) reporter
+       formatError
+         source maps
+           Windows
+             should correct rewrite stack traces with sha:
+      Uncaught AssertionError: expected 'at C:/a/b/c.js:2:6\n' to equal 'at c:/original/b.js:4:8 &lt;- C:/a/b/c.js:2:6\n'
+      + expected - actual
+      -at C:/a/b/c.js:2:6
+      +at c:/original/b.js:4:8 &lt;- C:/a/b/c.js:2:6
+      at test/unit/reporter.spec.js:379:43
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)</t>
+  </si>
+  <si>
+    <t>1) reporter
+       formatError
+         source maps
+           should rewrite stack traces to the first column when no column is given:
+      Uncaught AssertionError: expected 'at b.js:2\n' to equal 'at /original/b.js:4:3 &lt;- b.js:2\n'
+      + expected - actual
+      -at b.js:2
+      +at /original/b.js:4:3 &lt;- b.js:2
+      at test/unit/reporter.spec.js:273:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1) reporter
+       formatError
+         source maps
+           should not try to use source maps when no line is given:
+      Uncaught AssertionError: expected 'at /original/b.js:3 &lt;- b.js\n' to equal 'at b.js\n'
+      + expected - actual
+      -at /original/b.js:3 &lt;- b.js
+      +at b.js
+      at test/unit/reporter.spec.js:333:41
+      at Timeout._onTimeout (node_modules/lodash/lodash.js:2792:43)
+      at listOnTimeout (node:internal/timers:581:17)
+      at process.processTimers (node:internal/timers:519:7)</t>
+  </si>
+  <si>
+    <t>11 test  failures, 1 of which is the same as the one caused by the original bug</t>
   </si>
 </sst>
 </file>
@@ -367,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,9 +746,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -501,6 +832,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -835,34 +1181,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A505AA0-B029-1B43-BAF3-41DF5F895608}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="65.33203125" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="272">
+      <c r="A2" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="48">
+        <v>55</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C302C4E-966E-E54E-A26B-052C43363DBC}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="39.6640625" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="79" customWidth="1"/>
-    <col min="5" max="5" width="32.5" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="7" width="75.6640625" customWidth="1"/>
-    <col min="8" max="8" width="33.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
-    <col min="10" max="10" width="79.6640625" customWidth="1"/>
-    <col min="11" max="11" width="36" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" customWidth="1"/>
-    <col min="13" max="13" width="88" customWidth="1"/>
-    <col min="14" max="14" width="24.5" customWidth="1"/>
-    <col min="15" max="15" width="15.5" customWidth="1"/>
-    <col min="16" max="16" width="64.83203125" customWidth="1"/>
-    <col min="17" max="17" width="38.5" customWidth="1"/>
+    <col min="4" max="5" width="79" customWidth="1"/>
+    <col min="6" max="6" width="32.5" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="8" max="9" width="75.6640625" customWidth="1"/>
+    <col min="10" max="10" width="33.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="12" max="13" width="79.6640625" customWidth="1"/>
+    <col min="14" max="14" width="36" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" customWidth="1"/>
+    <col min="16" max="17" width="88" customWidth="1"/>
+    <col min="18" max="18" width="24.5" customWidth="1"/>
+    <col min="19" max="19" width="15.5" customWidth="1"/>
+    <col min="20" max="21" width="64.83203125" customWidth="1"/>
+    <col min="22" max="22" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:22">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -870,32 +1276,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="1"/>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="47" t="s">
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="41" t="s">
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="42" t="s">
         <v>7</v>
-      </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="42" t="s">
-        <v>8</v>
       </c>
       <c r="P1" s="42"/>
       <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:22">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="1"/>
@@ -903,50 +1314,63 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="G2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="M2" s="7"/>
+      <c r="N2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="10" t="s">
+      <c r="O2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="Q2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="8" t="s">
+      <c r="S2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="U2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="V2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="196" customHeight="1">
-      <c r="A3" s="45">
+    <row r="3" spans="1:22" ht="196" customHeight="1">
+      <c r="A3" s="44">
         <v>4</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="43" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="14">
@@ -956,48 +1380,63 @@
         <v>11</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="22">
+        <v>37</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="21">
         <v>1</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="H3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="27">
+      <c r="I3" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="26">
         <v>1</v>
       </c>
-      <c r="J3" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="35">
+      <c r="L3" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="34">
         <v>1</v>
       </c>
-      <c r="M3" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="36">
+      <c r="P3" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="35">
         <v>1</v>
       </c>
-      <c r="P3" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="40" t="s">
-        <v>25</v>
+      <c r="T3" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="U3" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" s="39" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="223" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="44"/>
+    <row r="4" spans="1:22" ht="223" customHeight="1">
+      <c r="A4" s="44"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="14">
         <v>2</v>
       </c>
@@ -1005,124 +1444,157 @@
         <v>12</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="23">
-        <v>2</v>
-      </c>
-      <c r="G4" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="22">
+        <v>2</v>
+      </c>
+      <c r="H4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="28">
-        <v>2</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="12" t="s">
+      <c r="I4" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="27">
+        <v>2</v>
+      </c>
+      <c r="L4" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="34">
+        <v>2</v>
+      </c>
+      <c r="P4" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" s="35">
+        <v>2</v>
+      </c>
+      <c r="T4" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="35">
-        <v>2</v>
-      </c>
-      <c r="M4" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="36">
-        <v>2</v>
-      </c>
-      <c r="P4" s="37" t="s">
+      <c r="U4" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="40" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="5" spans="1:17" ht="217" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="44"/>
+    <row r="5" spans="1:22" ht="217" customHeight="1">
+      <c r="A5" s="44"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="14">
         <v>3</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="22">
+        <v>3</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="30"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="34">
+        <v>3</v>
+      </c>
+      <c r="P5" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="23">
+      <c r="Q5" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="S5" s="35">
         <v>3</v>
       </c>
-      <c r="G5" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="35">
-        <v>3</v>
-      </c>
-      <c r="M5" s="34" t="s">
+      <c r="T5" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="36">
-        <v>3</v>
-      </c>
-      <c r="P5" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q5" s="40" t="s">
-        <v>27</v>
+      <c r="U5" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="169" customHeight="1">
-      <c r="A6" s="45"/>
-      <c r="B6" s="44"/>
+    <row r="6" spans="1:22" ht="169" customHeight="1">
+      <c r="A6" s="44"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="26"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="38"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="37"/>
     </row>
-    <row r="7" spans="1:17" ht="157" customHeight="1">
+    <row r="7" spans="1:22" ht="157" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="14">
@@ -1131,284 +1603,334 @@
       <c r="D7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="24">
+      <c r="E7" s="17"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="23">
         <v>5</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="36">
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="35">
         <v>5</v>
       </c>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="38"/>
+      <c r="T7" s="36"/>
+      <c r="U7" s="36"/>
+      <c r="V7" s="37"/>
     </row>
-    <row r="8" spans="1:17" ht="168" customHeight="1">
+    <row r="8" spans="1:22" ht="168" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="14">
         <v>6</v>
       </c>
       <c r="D8" s="17"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="25">
+      <c r="E8" s="17"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="24">
         <v>6</v>
       </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="31"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="36">
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="35">
         <v>6</v>
       </c>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="39"/>
+      <c r="T8" s="36"/>
+      <c r="U8" s="36"/>
+      <c r="V8" s="38"/>
     </row>
-    <row r="9" spans="1:17" ht="150" customHeight="1">
+    <row r="9" spans="1:22" ht="150" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="14">
         <v>7</v>
       </c>
       <c r="D9" s="17"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="25">
+      <c r="E9" s="17"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="24">
         <v>7</v>
       </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="36">
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="33"/>
+      <c r="S9" s="35">
         <v>7</v>
       </c>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="39"/>
+      <c r="T9" s="39"/>
+      <c r="U9" s="39"/>
+      <c r="V9" s="38"/>
     </row>
-    <row r="10" spans="1:17" ht="22">
+    <row r="10" spans="1:22" ht="22">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="14">
         <v>8</v>
       </c>
       <c r="D10" s="17"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="25">
+      <c r="E10" s="17"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="24">
         <v>8</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="36">
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="35">
         <v>8</v>
       </c>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="39"/>
+      <c r="T10" s="39"/>
+      <c r="U10" s="39"/>
+      <c r="V10" s="38"/>
     </row>
-    <row r="11" spans="1:17" ht="22">
+    <row r="11" spans="1:22" ht="22">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="14">
         <v>9</v>
       </c>
       <c r="D11" s="17"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="25">
+      <c r="E11" s="17"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="24">
         <v>9</v>
       </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="31"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="36">
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="35">
         <v>9</v>
       </c>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="39"/>
+      <c r="T11" s="39"/>
+      <c r="U11" s="39"/>
+      <c r="V11" s="38"/>
     </row>
-    <row r="12" spans="1:17" ht="22">
+    <row r="12" spans="1:22" ht="22">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="14">
         <v>10</v>
       </c>
       <c r="D12" s="17"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="25">
+      <c r="E12" s="17"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="24">
         <v>10</v>
       </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="31"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="36">
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="35">
         <v>10</v>
       </c>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="39"/>
+      <c r="T12" s="39"/>
+      <c r="U12" s="39"/>
+      <c r="V12" s="38"/>
     </row>
-    <row r="13" spans="1:17" ht="22">
+    <row r="13" spans="1:22" ht="22">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="14">
         <v>11</v>
       </c>
       <c r="D13" s="17"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="25">
+      <c r="E13" s="17"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="24">
         <v>11</v>
       </c>
-      <c r="G13" s="26"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="31"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="36">
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="35">
         <v>11</v>
       </c>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="39"/>
+      <c r="T13" s="39"/>
+      <c r="U13" s="39"/>
+      <c r="V13" s="38"/>
     </row>
-    <row r="14" spans="1:17" ht="22">
+    <row r="14" spans="1:22" ht="22">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="14">
         <v>12</v>
       </c>
       <c r="D14" s="17"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="25">
+      <c r="E14" s="17"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="24">
         <v>12</v>
       </c>
-      <c r="G14" s="26"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="31"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="33"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:22">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="6"/>
+      <c r="F15" s="2"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="32"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
       <c r="K15" s="12"/>
-      <c r="L15" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:22">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="6"/>
+      <c r="F16" s="2"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
       <c r="K16" s="12"/>
-      <c r="L16" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="M16" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="N16" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="P16" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="O1:R1"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="A3:A6"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>